<commit_message>
8/5 Project System: Config.jsg
</commit_message>
<xml_diff>
--- a/example/test1.xlsx
+++ b/example/test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio\Projects\JSONGenerator\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C4A936-150F-41FA-8FA1-2FEED4B21831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809ED7CA-1527-4DE4-A354-46EA5309DB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3619" yWindow="2054" windowWidth="18745" windowHeight="14162" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7738" yWindow="1440" windowWidth="22064" windowHeight="14162" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testSheet1" sheetId="1" r:id="rId1"/>
@@ -584,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="A1:N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -673,79 +673,79 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F5" s="3">
         <v>13.25</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L3">
+      <c r="L5">
         <v>23</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F6" s="3">
         <v>133</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L4">
+      <c r="L6">
         <v>39</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -759,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E86084-205F-441B-89FA-3DB6B2E9435C}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>